<commit_message>
updated stats and costs sheets
</commit_message>
<xml_diff>
--- a/cam/ADS1299-shield-bom.xlsx
+++ b/cam/ADS1299-shield-bom.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="212">
   <si>
     <t>Reference</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Components</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>PCB</t>
   </si>
   <si>
@@ -233,9 +230,6 @@
     <t>PIN HEADER - 5V-2.5V - 1x3 male header</t>
   </si>
   <si>
-    <t>PIN HEADER - PWMH - 1x10 female header</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -257,9 +251,6 @@
     <t>TPS73225DBVT - Cap-Free, NMOS, 250mA Low Dropout Regulator</t>
   </si>
   <si>
-    <t>ADS1299IPAG - 8-Channel, 24-Bit Analog-To-Digital Converter With Integrated EEG Front End.</t>
-  </si>
-  <si>
     <t>Size</t>
   </si>
   <si>
@@ -461,15 +452,6 @@
     <t>A113802-ND</t>
   </si>
   <si>
-    <t>SMT?</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>NI</t>
   </si>
   <si>
@@ -488,9 +470,6 @@
     <t>Pins extension</t>
   </si>
   <si>
-    <t>Total components</t>
-  </si>
-  <si>
     <t>CL10A225KP8NNNC</t>
   </si>
   <si>
@@ -539,9 +518,6 @@
     <t>Microchip</t>
   </si>
   <si>
-    <t>ADS1299IPAG</t>
-  </si>
-  <si>
     <t>TPS72325DBVT</t>
   </si>
   <si>
@@ -612,6 +588,75 @@
   </si>
   <si>
     <t>http://www.4uconnector.com/online/SearchPro.asp?FormName=ProSearch&amp;FormAction=search&amp;s_GroupNo=&amp;s_keyword=18677</t>
+  </si>
+  <si>
+    <t>JP18</t>
+  </si>
+  <si>
+    <t>PIN HEADER - 1x10 female header</t>
+  </si>
+  <si>
+    <t>PIN HEADER - 2x18 female header</t>
+  </si>
+  <si>
+    <t>http://www.4uconnector.com/online/SearchPro.asp?FormName=ProSearch&amp;FormAction=search&amp;s_GroupNo=&amp;s_keyword=19639</t>
+  </si>
+  <si>
+    <t>Shipping</t>
+  </si>
+  <si>
+    <t>my margin</t>
+  </si>
+  <si>
+    <t>distributor cost</t>
+  </si>
+  <si>
+    <t>distributor margin</t>
+  </si>
+  <si>
+    <t>end user cost</t>
+  </si>
+  <si>
+    <t>Conservative</t>
+  </si>
+  <si>
+    <t>Bigger</t>
+  </si>
+  <si>
+    <t>BOM line items</t>
+  </si>
+  <si>
+    <t>Though-hole pins</t>
+  </si>
+  <si>
+    <t>Pins/Pads</t>
+  </si>
+  <si>
+    <t>ADS1299CPAG - 8-Channel, 24-Bit Analog-To-Digital Converter With Integrated EEG Front End.</t>
+  </si>
+  <si>
+    <t>ADS1299CPAG</t>
+  </si>
+  <si>
+    <t>SMT/TH</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>TQFP64</t>
+  </si>
+  <si>
+    <t>SOT23-5</t>
+  </si>
+  <si>
+    <t>SOIC-8</t>
+  </si>
+  <si>
+    <t>SMT Pads</t>
+  </si>
+  <si>
+    <t>Total component items</t>
   </si>
 </sst>
 </file>
@@ -708,7 +753,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -733,6 +778,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1086,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1109,13 +1156,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>146</v>
+        <v>205</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -1127,19 +1174,19 @@
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="I1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="45">
@@ -1147,28 +1194,35 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G2">
         <v>3</v>
       </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I17" si="0">G2*H2</f>
+        <v>6</v>
+      </c>
       <c r="J2" t="s">
         <v>5</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1176,57 +1230,71 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="E3" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="J3" t="s">
         <v>7</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="E4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G4">
         <v>7</v>
       </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
       <c r="J4" t="s">
         <v>8</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30">
@@ -1234,31 +1302,38 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="E5" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G5">
         <v>17</v>
       </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
       <c r="J5" t="s">
         <v>10</v>
       </c>
       <c r="K5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45">
@@ -1266,28 +1341,35 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E6" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6">
         <v>25</v>
       </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
       <c r="J6" t="s">
         <v>12</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30">
@@ -1295,86 +1377,107 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E7" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7">
         <v>12</v>
       </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
       <c r="J7" t="s">
         <v>14</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E8" t="s">
+        <v>160</v>
+      </c>
+      <c r="F8" t="s">
         <v>90</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E8" t="s">
-        <v>167</v>
-      </c>
-      <c r="F8" t="s">
-        <v>93</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="J8" t="s">
+        <v>86</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E9" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="F9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="J9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1382,25 +1485,35 @@
         <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="E10" t="s">
-        <v>172</v>
+        <v>204</v>
       </c>
       <c r="F10" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G10">
         <v>1</v>
       </c>
+      <c r="H10">
+        <v>64</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
       <c r="J10" t="s">
-        <v>78</v>
+        <v>203</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1408,25 +1521,35 @@
         <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="E11" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="F11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="J11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1434,25 +1557,35 @@
         <v>17</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>208</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="F12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="J12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1460,25 +1593,35 @@
         <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E13" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="F13" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
+      <c r="H13">
+        <v>8</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="J13" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1486,25 +1629,35 @@
         <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>208</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="E14" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="F14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="J14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1512,25 +1665,35 @@
         <v>20</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>208</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="E15" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="F15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G15">
         <v>2</v>
       </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="J15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1538,25 +1701,35 @@
         <v>21</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>208</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="E16" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="F16" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
+      <c r="H16">
+        <v>8</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="J16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1564,25 +1737,32 @@
         <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D17" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E17" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G17">
         <v>1</v>
       </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="J17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1590,16 +1770,16 @@
         <v>23</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E18" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="F18" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1612,10 +1792,10 @@
         <v>30</v>
       </c>
       <c r="J18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1623,16 +1803,16 @@
         <v>24</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="D19" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E19" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="F19" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1641,14 +1821,14 @@
         <v>8</v>
       </c>
       <c r="I19">
-        <f t="shared" ref="I19:I24" si="0">G19*H19</f>
+        <f t="shared" ref="I19:I24" si="1">G19*H19</f>
         <v>8</v>
       </c>
       <c r="J19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1656,16 +1836,16 @@
         <v>25</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="D20" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E20" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="F20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1674,25 +1854,25 @@
         <v>24</v>
       </c>
       <c r="I20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="J20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E21">
         <v>18689</v>
@@ -1704,14 +1884,14 @@
         <v>8</v>
       </c>
       <c r="I21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="J21" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1719,16 +1899,16 @@
         <v>26</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="D22" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E22" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="F22" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1737,31 +1917,31 @@
         <v>20</v>
       </c>
       <c r="I22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="J22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="D23" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="E23" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1770,17 +1950,17 @@
         <v>15</v>
       </c>
       <c r="I23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="J23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1788,10 +1968,10 @@
         <v>27</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>148</v>
+        <v>206</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E24">
         <v>19950</v>
@@ -1803,69 +1983,80 @@
         <v>10</v>
       </c>
       <c r="I24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="J24" t="s">
-        <v>70</v>
+        <v>190</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="2" t="s">
-        <v>28</v>
+        <v>189</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>147</v>
+        <v>206</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>161</v>
-      </c>
-      <c r="E25" t="s">
-        <v>188</v>
-      </c>
-      <c r="F25" t="s">
-        <v>112</v>
+        <v>71</v>
+      </c>
+      <c r="E25">
+        <v>19950</v>
       </c>
       <c r="G25">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>36</v>
+      </c>
+      <c r="I25">
+        <f t="shared" ref="I25:I35" si="2">G25*H25</f>
+        <v>36</v>
       </c>
       <c r="J25" t="s">
-        <v>29</v>
+        <v>191</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>113</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="E26" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="F26" t="s">
         <v>109</v>
       </c>
       <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
         <v>2</v>
       </c>
+      <c r="I26">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
       <c r="J26" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L26" s="3" t="s">
         <v>110</v>
@@ -1873,203 +2064,265 @@
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="E27" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="F27" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G27">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="J27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E28" t="s">
+        <v>183</v>
+      </c>
+      <c r="F28" t="s">
+        <v>100</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="J28" t="s">
+        <v>33</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" t="s">
-        <v>190</v>
-      </c>
-      <c r="E28" t="s">
-        <v>192</v>
-      </c>
-      <c r="F28" t="s">
-        <v>107</v>
-      </c>
-      <c r="G28">
+      <c r="B29" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" t="s">
+        <v>182</v>
+      </c>
+      <c r="E29" t="s">
+        <v>184</v>
+      </c>
+      <c r="F29" t="s">
+        <v>104</v>
+      </c>
+      <c r="G29">
         <v>2</v>
       </c>
-      <c r="J28" t="s">
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J29" t="s">
         <v>35</v>
       </c>
-      <c r="L28" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="45">
-      <c r="A29" s="2" t="s">
+      <c r="L29" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="45">
+      <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" t="s">
-        <v>190</v>
-      </c>
-      <c r="E29" t="s">
-        <v>193</v>
-      </c>
-      <c r="F29" t="s">
-        <v>102</v>
-      </c>
-      <c r="G29">
+      <c r="B30" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" t="s">
+        <v>182</v>
+      </c>
+      <c r="E30" t="s">
+        <v>185</v>
+      </c>
+      <c r="F30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G30">
         <v>18</v>
       </c>
-      <c r="J29" t="s">
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="J30" t="s">
         <v>37</v>
       </c>
-      <c r="L29" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E30">
-        <v>18677</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-      <c r="J30" t="s">
-        <v>39</v>
-      </c>
-      <c r="L30" t="s">
-        <v>196</v>
+      <c r="L30" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>149</v>
+        <v>206</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31">
+        <v>18677</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>6</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="J31" t="s">
-        <v>41</v>
-      </c>
-      <c r="K31" t="s">
-        <v>111</v>
+        <v>39</v>
+      </c>
+      <c r="L31" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="J32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="J33" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K33" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J34" t="s">
+        <v>45</v>
+      </c>
+      <c r="K34" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="E34" t="s">
-        <v>194</v>
-      </c>
-      <c r="F34" t="s">
-        <v>130</v>
-      </c>
-      <c r="G34">
+      <c r="B35" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="E35" t="s">
+        <v>186</v>
+      </c>
+      <c r="F35" t="s">
+        <v>127</v>
+      </c>
+      <c r="G35">
         <v>2</v>
       </c>
-      <c r="J34" t="s">
-        <v>85</v>
-      </c>
-      <c r="L34" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="6"/>
+      <c r="H35">
+        <v>20</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="J35" t="s">
+        <v>82</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="40" spans="1:12">
-      <c r="B40" s="5"/>
+      <c r="A40" s="6"/>
     </row>
     <row r="41" spans="1:12">
       <c r="B41" s="5"/>
     </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="6"/>
-      <c r="B43" s="5"/>
+    <row r="42" spans="1:12">
+      <c r="B42" s="5"/>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="6"/>
+      <c r="B44" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2080,11 +2333,11 @@
     <hyperlink ref="L3" r:id="rId5"/>
     <hyperlink ref="L5" r:id="rId6"/>
     <hyperlink ref="L17" r:id="rId7"/>
-    <hyperlink ref="L29" r:id="rId8"/>
-    <hyperlink ref="L27" r:id="rId9"/>
-    <hyperlink ref="L28" r:id="rId10"/>
-    <hyperlink ref="L26" r:id="rId11"/>
-    <hyperlink ref="L25" r:id="rId12"/>
+    <hyperlink ref="L30" r:id="rId8"/>
+    <hyperlink ref="L28" r:id="rId9"/>
+    <hyperlink ref="L29" r:id="rId10"/>
+    <hyperlink ref="L27" r:id="rId11"/>
+    <hyperlink ref="L26" r:id="rId12"/>
     <hyperlink ref="L10" r:id="rId13"/>
     <hyperlink ref="L11" r:id="rId14"/>
     <hyperlink ref="L12" r:id="rId15"/>
@@ -2092,7 +2345,7 @@
     <hyperlink ref="L14" r:id="rId17"/>
     <hyperlink ref="L15" r:id="rId18"/>
     <hyperlink ref="L16" r:id="rId19"/>
-    <hyperlink ref="L34" r:id="rId20"/>
+    <hyperlink ref="L35" r:id="rId20"/>
     <hyperlink ref="L18" r:id="rId21"/>
     <hyperlink ref="L19" r:id="rId22"/>
     <hyperlink ref="L20" r:id="rId23"/>
@@ -2100,8 +2353,8 @@
     <hyperlink ref="L22" r:id="rId25"/>
     <hyperlink ref="L24" r:id="rId26"/>
     <hyperlink ref="D9" r:id="rId27"/>
-    <hyperlink ref="D26" r:id="rId28"/>
-    <hyperlink ref="D27:D29" r:id="rId29" display="Panasonic Electronic Components"/>
+    <hyperlink ref="D27" r:id="rId28"/>
+    <hyperlink ref="D28:D30" r:id="rId29" display="Panasonic Electronic Components"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2115,73 +2368,157 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="3" spans="1:3">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>52</v>
       </c>
       <c r="B5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>50</v>
       </c>
       <c r="B6">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>75</v>
+      </c>
+      <c r="C6">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>47</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="10">
         <f>SUM(B5:B9)</f>
-        <v>127</v>
+        <v>125</v>
+      </c>
+      <c r="C11" s="10">
+        <f>SUM(C5:C9)</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>194</v>
+      </c>
+      <c r="B15">
+        <v>0.5</v>
+      </c>
+      <c r="C15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>195</v>
+      </c>
+      <c r="B17" s="10">
+        <f>B11+B11*B15</f>
+        <v>187.5</v>
+      </c>
+      <c r="C17" s="10">
+        <f>C11+C11*C15</f>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>196</v>
+      </c>
+      <c r="B18">
+        <v>0.5</v>
+      </c>
+      <c r="C18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20">
+        <f>B17+B17*B18</f>
+        <v>281.25</v>
+      </c>
+      <c r="C20">
+        <f>C17+C17*C18</f>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2192,10 +2529,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2205,48 +2542,73 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B2" s="8">
+        <f>SUMIF(BOM!B2:B35,"=SMT",BOM!G2:G35)</f>
         <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B3" s="8">
-        <v>13</v>
+        <f>SUMIF(BOM!B3:B36,"=TH",BOM!G3:G36)</f>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+      <c r="B4" s="8"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B5" s="8">
+        <v>202</v>
+      </c>
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B6" s="8">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" s="8">
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B8">
-        <f>SUM(BOM!G2:G35)</f>
-        <v>123</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+    <row r="9" spans="1:4">
+      <c r="A9" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B9">
+        <f>COUNT(BOM!G2:G35)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10">
+        <f>SUM(BOM!G2:G36)</f>
+        <v>124</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated BOM with new and changed parts - needs to be checked once more
</commit_message>
<xml_diff>
--- a/cam/ADS1299-shield-bom.xlsx
+++ b/cam/ADS1299-shield-bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16620" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="216">
   <si>
     <t>Reference</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Capacitor - 2.2uF</t>
   </si>
   <si>
-    <t>C17</t>
-  </si>
-  <si>
     <t>Capacitor - 100uF</t>
   </si>
   <si>
@@ -218,15 +215,9 @@
     <t>PIN HEADER - CONFIG1 - 2x12 male header</t>
   </si>
   <si>
-    <t>PIN HEADER - BOARD_ADDRESS - 2x4 male header</t>
-  </si>
-  <si>
     <t>PIN HEADER - Electrode Connector - 2x15 RA male shrouded header</t>
   </si>
   <si>
-    <t>PIN HEADER - CONFIG3 - 2x10 male header</t>
-  </si>
-  <si>
     <t>PIN HEADER - 5V-2.5V - 1x3 male header</t>
   </si>
   <si>
@@ -305,9 +296,6 @@
     <t>160-1737-1-ND</t>
   </si>
   <si>
-    <t>adafruit :: JST_3PIN PH Series - EXTERNAL_SYNC</t>
-  </si>
-  <si>
     <t>http://www.digikey.com/product-search/en?mpart=S3B-PH-K-S%28LF%29%28SN%29&amp;vendor=455</t>
   </si>
   <si>
@@ -657,6 +645,30 @@
   </si>
   <si>
     <t>Total component items</t>
+  </si>
+  <si>
+    <t>PIN HEADER - 2x4 male header</t>
+  </si>
+  <si>
+    <t>JST_3PIN - PH Series</t>
+  </si>
+  <si>
+    <t>PIN HEADER - 2x10 male header</t>
+  </si>
+  <si>
+    <t>C17, C25</t>
+  </si>
+  <si>
+    <t>P392HCT-ND</t>
+  </si>
+  <si>
+    <t>Resistor - 392</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/ERJ-3EKF3920V/P392HCT-ND/198363</t>
+  </si>
+  <si>
+    <t>R6</t>
   </si>
 </sst>
 </file>
@@ -728,7 +740,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -737,6 +749,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -781,7 +794,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="24">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -800,6 +813,7 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1133,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1156,37 +1170,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
       </c>
       <c r="H1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="I1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="45">
@@ -1194,91 +1208,91 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I17" si="0">G2*H2</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J2" t="s">
         <v>5</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>211</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G4">
         <v>7</v>
@@ -1291,30 +1305,30 @@
         <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G5">
         <v>17</v>
@@ -1327,105 +1341,105 @@
         <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="45">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E6" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G6">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H6">
         <v>2</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G7">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H7">
         <v>2</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="30">
       <c r="A8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F8" t="s">
         <v>87</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E8" t="s">
-        <v>160</v>
-      </c>
-      <c r="F8" t="s">
-        <v>90</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1438,30 +1452,30 @@
         <v>2</v>
       </c>
       <c r="J8" t="s">
+        <v>83</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E9" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -1474,30 +1488,30 @@
         <v>2</v>
       </c>
       <c r="J9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E10" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1510,30 +1524,30 @@
         <v>64</v>
       </c>
       <c r="J10" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -1546,30 +1560,30 @@
         <v>5</v>
       </c>
       <c r="J11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F12" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1582,30 +1596,30 @@
         <v>5</v>
       </c>
       <c r="J12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E13" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F13" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1618,30 +1632,30 @@
         <v>8</v>
       </c>
       <c r="J13" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E14" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1654,30 +1668,30 @@
         <v>5</v>
       </c>
       <c r="J14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E15" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -1690,30 +1704,30 @@
         <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E16" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -1726,27 +1740,27 @@
         <v>8</v>
       </c>
       <c r="J16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D17" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -1759,27 +1773,27 @@
         <v>2</v>
       </c>
       <c r="J17" t="s">
-        <v>94</v>
+        <v>209</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E18" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F18" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1792,27 +1806,27 @@
         <v>30</v>
       </c>
       <c r="J18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D19" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E19" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F19" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -1825,27 +1839,27 @@
         <v>8</v>
       </c>
       <c r="J19" t="s">
-        <v>65</v>
+        <v>208</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D20" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E20" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F20" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1858,21 +1872,21 @@
         <v>24</v>
       </c>
       <c r="J20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E21">
         <v>18689</v>
@@ -1888,27 +1902,27 @@
         <v>48</v>
       </c>
       <c r="J21" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D22" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E22" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F22" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -1921,27 +1935,27 @@
         <v>20</v>
       </c>
       <c r="J22" t="s">
-        <v>67</v>
+        <v>210</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D23" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E23" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F23" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -1954,24 +1968,24 @@
         <v>15</v>
       </c>
       <c r="J23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K23" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D24" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E24">
         <v>19950</v>
@@ -1987,24 +2001,24 @@
         <v>10</v>
       </c>
       <c r="J24" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E25">
         <v>19950</v>
@@ -2016,34 +2030,34 @@
         <v>36</v>
       </c>
       <c r="I25">
-        <f t="shared" ref="I25:I35" si="2">G25*H25</f>
+        <f t="shared" ref="I25:I36" si="2">G25*H25</f>
         <v>36</v>
       </c>
       <c r="J25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D26" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E26" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="F26" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G26">
         <v>4</v>
@@ -2056,30 +2070,30 @@
         <v>8</v>
       </c>
       <c r="J26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D27" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E27" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G27">
         <v>2</v>
@@ -2092,237 +2106,273 @@
         <v>4</v>
       </c>
       <c r="J27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" s="2" t="s">
-        <v>32</v>
+        <v>215</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E28" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F28" t="s">
-        <v>100</v>
+        <v>212</v>
       </c>
       <c r="G28">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <v>2</v>
       </c>
       <c r="I28">
+        <f t="shared" ref="I28" si="3">G28*H28</f>
+        <v>2</v>
+      </c>
+      <c r="J28" t="s">
+        <v>213</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" t="s">
+        <v>178</v>
+      </c>
+      <c r="E29" t="s">
+        <v>179</v>
+      </c>
+      <c r="F29" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29">
+        <v>6</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J29" t="s">
+        <v>32</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="L28" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" t="s">
-        <v>182</v>
-      </c>
-      <c r="E29" t="s">
-        <v>184</v>
-      </c>
-      <c r="F29" t="s">
-        <v>104</v>
-      </c>
-      <c r="G29">
+      <c r="B30" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" t="s">
+        <v>178</v>
+      </c>
+      <c r="E30" t="s">
+        <v>180</v>
+      </c>
+      <c r="F30" t="s">
+        <v>100</v>
+      </c>
+      <c r="G30">
         <v>2</v>
       </c>
-      <c r="H29">
+      <c r="H30">
         <v>2</v>
       </c>
-      <c r="I29">
+      <c r="I30">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J30" t="s">
+        <v>34</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="45">
+      <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L29" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="45">
-      <c r="A30" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D30" t="s">
-        <v>182</v>
-      </c>
-      <c r="E30" t="s">
-        <v>185</v>
-      </c>
-      <c r="F30" t="s">
-        <v>99</v>
-      </c>
-      <c r="G30">
+      <c r="B31" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" t="s">
+        <v>178</v>
+      </c>
+      <c r="E31" t="s">
+        <v>181</v>
+      </c>
+      <c r="F31" t="s">
+        <v>95</v>
+      </c>
+      <c r="G31">
         <v>18</v>
       </c>
-      <c r="H30">
+      <c r="H31">
         <v>2</v>
       </c>
-      <c r="I30">
+      <c r="I31">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J31" t="s">
+        <v>36</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L30" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E31">
+      <c r="B32" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32">
         <v>18677</v>
       </c>
-      <c r="G31">
+      <c r="G32">
         <v>1</v>
       </c>
-      <c r="H31">
+      <c r="H32">
         <v>6</v>
       </c>
-      <c r="I31">
+      <c r="I32">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="J31" t="s">
-        <v>39</v>
-      </c>
-      <c r="L31" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>143</v>
-      </c>
       <c r="J32" t="s">
-        <v>41</v>
-      </c>
-      <c r="K32" t="s">
-        <v>108</v>
+        <v>38</v>
+      </c>
+      <c r="L32" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="A33" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J33" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="K33" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J34" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K34" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:12">
       <c r="A35" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="E35" t="s">
-        <v>186</v>
-      </c>
-      <c r="F35" t="s">
-        <v>127</v>
-      </c>
-      <c r="G35">
+        <v>139</v>
+      </c>
+      <c r="J35" t="s">
+        <v>44</v>
+      </c>
+      <c r="K35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="E36" t="s">
+        <v>182</v>
+      </c>
+      <c r="F36" t="s">
+        <v>123</v>
+      </c>
+      <c r="G36">
         <v>2</v>
       </c>
-      <c r="H35">
+      <c r="H36">
         <v>20</v>
       </c>
-      <c r="I35">
+      <c r="I36">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="J35" t="s">
-        <v>82</v>
-      </c>
-      <c r="L35" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="A40" s="6"/>
+      <c r="J36" t="s">
+        <v>79</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="41" spans="1:12">
-      <c r="B41" s="5"/>
+      <c r="A41" s="6"/>
     </row>
     <row r="42" spans="1:12">
       <c r="B42" s="5"/>
     </row>
-    <row r="44" spans="1:12">
-      <c r="A44" s="6"/>
-      <c r="B44" s="5"/>
+    <row r="43" spans="1:12">
+      <c r="B43" s="5"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="6"/>
+      <c r="B45" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2333,28 +2383,29 @@
     <hyperlink ref="L3" r:id="rId5"/>
     <hyperlink ref="L5" r:id="rId6"/>
     <hyperlink ref="L17" r:id="rId7"/>
-    <hyperlink ref="L30" r:id="rId8"/>
-    <hyperlink ref="L28" r:id="rId9"/>
-    <hyperlink ref="L29" r:id="rId10"/>
-    <hyperlink ref="L27" r:id="rId11"/>
-    <hyperlink ref="L26" r:id="rId12"/>
-    <hyperlink ref="L10" r:id="rId13"/>
-    <hyperlink ref="L11" r:id="rId14"/>
-    <hyperlink ref="L12" r:id="rId15"/>
-    <hyperlink ref="L13" r:id="rId16"/>
-    <hyperlink ref="L14" r:id="rId17"/>
-    <hyperlink ref="L15" r:id="rId18"/>
-    <hyperlink ref="L16" r:id="rId19"/>
-    <hyperlink ref="L35" r:id="rId20"/>
-    <hyperlink ref="L18" r:id="rId21"/>
-    <hyperlink ref="L19" r:id="rId22"/>
-    <hyperlink ref="L20" r:id="rId23"/>
-    <hyperlink ref="L23" r:id="rId24"/>
-    <hyperlink ref="L22" r:id="rId25"/>
-    <hyperlink ref="L24" r:id="rId26"/>
-    <hyperlink ref="D9" r:id="rId27"/>
-    <hyperlink ref="D27" r:id="rId28"/>
-    <hyperlink ref="D28:D30" r:id="rId29" display="Panasonic Electronic Components"/>
+    <hyperlink ref="L31" r:id="rId8"/>
+    <hyperlink ref="L30" r:id="rId9"/>
+    <hyperlink ref="L27" r:id="rId10"/>
+    <hyperlink ref="L26" r:id="rId11"/>
+    <hyperlink ref="L10" r:id="rId12"/>
+    <hyperlink ref="L11" r:id="rId13"/>
+    <hyperlink ref="L12" r:id="rId14"/>
+    <hyperlink ref="L13" r:id="rId15"/>
+    <hyperlink ref="L14" r:id="rId16"/>
+    <hyperlink ref="L15" r:id="rId17"/>
+    <hyperlink ref="L16" r:id="rId18"/>
+    <hyperlink ref="L36" r:id="rId19"/>
+    <hyperlink ref="L18" r:id="rId20"/>
+    <hyperlink ref="L19" r:id="rId21"/>
+    <hyperlink ref="L20" r:id="rId22"/>
+    <hyperlink ref="L23" r:id="rId23"/>
+    <hyperlink ref="L22" r:id="rId24"/>
+    <hyperlink ref="L24" r:id="rId25"/>
+    <hyperlink ref="D9" r:id="rId26"/>
+    <hyperlink ref="D27" r:id="rId27"/>
+    <hyperlink ref="D29:D31" r:id="rId28" display="Panasonic Electronic Components"/>
+    <hyperlink ref="D28" r:id="rId29"/>
+    <hyperlink ref="L29" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2383,7 +2434,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2394,15 +2445,15 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -2413,7 +2464,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>75</v>
@@ -2424,7 +2475,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>35</v>
@@ -2435,7 +2486,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -2446,7 +2497,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -2457,7 +2508,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="10">
         <f>SUM(B5:B9)</f>
@@ -2470,7 +2521,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B15">
         <v>0.5</v>
@@ -2481,7 +2532,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B17" s="10">
         <f>B11+B11*B15</f>
@@ -2494,7 +2545,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B18">
         <v>0.5</v>
@@ -2505,7 +2556,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B20">
         <f>B17+B17*B18</f>
@@ -2542,25 +2593,25 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B2" s="8">
-        <f>SUMIF(BOM!B2:B35,"=SMT",BOM!G2:G35)</f>
-        <v>110</v>
+        <f>SUMIF(BOM!B2:B36,"=SMT",BOM!G2:G36)</f>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B3" s="8">
-        <f>SUMIF(BOM!B3:B36,"=TH",BOM!G3:G36)</f>
+        <f>SUMIF(BOM!B3:B37,"=TH",BOM!G3:G37)</f>
         <v>14</v>
       </c>
     </row>
@@ -2570,13 +2621,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B5" s="8"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B6" s="8">
         <v>148</v>
@@ -2584,7 +2635,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B7" s="8">
         <v>115</v>
@@ -2592,20 +2643,20 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B9">
-        <f>COUNT(BOM!G2:G35)</f>
-        <v>31</v>
+        <f>COUNT(BOM!G2:G36)</f>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="6" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B10">
-        <f>SUM(BOM!G2:G36)</f>
-        <v>124</v>
+        <f>SUM(BOM!G2:G37)</f>
+        <v>130</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>

</xml_diff>

<commit_message>
made lable text bigger and repositioned; added Arduino pin labels; added 1uf cap to 2.5 power supple to match eval board; relabeled power and buffer 3-pin jumpers with numbers instead of letters, to match schematic; adjusted autoroute of XIO connector rotation change; adjusted trace widths various places
</commit_message>
<xml_diff>
--- a/cam/ADS1299-shield-bom.xlsx
+++ b/cam/ADS1299-shield-bom.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="257">
   <si>
     <t>Reference</t>
   </si>
@@ -322,9 +322,6 @@
     <t>160-1737-1-ND</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-search/en?mpart=S3B-PH-K-S%28LF%29%28SN%29&amp;vendor=455</t>
-  </si>
-  <si>
     <t>455-1720-ND</t>
   </si>
   <si>
@@ -367,9 +364,6 @@
     <t>445-1019-1-ND</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/MLF1608A3R3K/445-1019-1-ND/504417</t>
-  </si>
-  <si>
     <t>296-34818-1-ND</t>
   </si>
   <si>
@@ -415,9 +409,6 @@
     <t>296-21978-1-ND</t>
   </si>
   <si>
-    <t>http://www.digikey.com/product-detail/en/TXS0102DCTR/296-21978-1-ND/1632671</t>
-  </si>
-  <si>
     <t>296-21527-1-ND</t>
   </si>
   <si>
@@ -821,6 +812,27 @@
   </si>
   <si>
     <t>0805</t>
+  </si>
+  <si>
+    <t>C7,C9,C11,C13,C15,C18,C19,C21,C22,C23,C26,C29,C30,C32,C50,C51,C52,C54,C56,C58,C60,C61,C65,C68,C70,C72</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/S3B-PH-SM4-TB(LF)(SN)/455-1750-1-ND/926847</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/MLZ2012A3R3W/445-6394-1-ND/2465720</t>
+  </si>
+  <si>
+    <t>TXS0102DCUR - 2-Bit Bi-Directional Level Shifter (I2C, etc.)</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/TXS0102DCUR/296-21931-1-ND/1629284</t>
+  </si>
+  <si>
+    <t>TXS0102DCUR</t>
+  </si>
+  <si>
+    <t>296-21931-1-ND</t>
   </si>
 </sst>
 </file>
@@ -1496,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:F16"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1517,7 +1529,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>70</v>
@@ -1532,13 +1544,13 @@
         <v>45</v>
       </c>
       <c r="G1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="H1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -1547,7 +1559,7 @@
         <v>63</v>
       </c>
       <c r="L1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="M1" t="s">
         <v>52</v>
@@ -1555,19 +1567,19 @@
     </row>
     <row r="2" spans="1:13" ht="45">
       <c r="A2" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>51</v>
@@ -1586,7 +1598,7 @@
         <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>53</v>
@@ -1594,22 +1606,22 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -1625,7 +1637,7 @@
         <v>6</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1633,16 +1645,16 @@
         <v>80</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>85</v>
@@ -1669,19 +1681,19 @@
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1694,10 +1706,10 @@
         <v>8</v>
       </c>
       <c r="J5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1705,19 +1717,19 @@
         <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -1733,7 +1745,7 @@
         <v>66</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1741,19 +1753,19 @@
         <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -1769,7 +1781,7 @@
         <v>68</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1777,19 +1789,19 @@
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -1805,7 +1817,7 @@
         <v>69</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1813,16 +1825,16 @@
         <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E9" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G9">
         <v>2</v>
@@ -1838,7 +1850,7 @@
         <v>74</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1846,19 +1858,19 @@
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>116</v>
+        <v>183</v>
+      </c>
+      <c r="D10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E10" t="s">
+        <v>255</v>
+      </c>
+      <c r="F10" t="s">
+        <v>256</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -1871,10 +1883,10 @@
         <v>8</v>
       </c>
       <c r="J10" t="s">
-        <v>67</v>
+        <v>253</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>117</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1882,19 +1894,19 @@
         <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>113</v>
+        <v>183</v>
+      </c>
+      <c r="D11" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F11" t="s">
+        <v>111</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -1907,10 +1919,10 @@
         <v>10</v>
       </c>
       <c r="J11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1918,19 +1930,19 @@
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1943,27 +1955,27 @@
         <v>64</v>
       </c>
       <c r="J12" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>58</v>
@@ -1987,22 +1999,22 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -2015,40 +2027,40 @@
         <v>4</v>
       </c>
       <c r="J14" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>216</v>
+        <v>250</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>56</v>
       </c>
       <c r="G15">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H15">
         <v>2</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J15" t="s">
         <v>10</v>
@@ -2062,19 +2074,19 @@
         <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G16">
         <v>4</v>
@@ -2090,24 +2102,24 @@
         <v>26</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>101</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>54</v>
@@ -2134,16 +2146,16 @@
         <v>19</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E18" t="s">
-        <v>248</v>
-      </c>
-      <c r="F18" t="s">
-        <v>247</v>
+        <v>154</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>244</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -2156,10 +2168,10 @@
         <v>2</v>
       </c>
       <c r="J18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>86</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="30">
@@ -2167,18 +2179,18 @@
         <v>79</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E19" t="s">
-        <v>145</v>
-      </c>
-      <c r="F19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>82</v>
       </c>
       <c r="G19">
@@ -2203,16 +2215,16 @@
         <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E20" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F20" t="s">
         <v>77</v>
@@ -2242,16 +2254,16 @@
         <v>22</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D21" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E21" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -2267,7 +2279,7 @@
         <v>60</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -2275,16 +2287,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D22" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E22" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F22" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -2297,10 +2309,10 @@
         <v>8</v>
       </c>
       <c r="J22" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -2308,16 +2320,16 @@
         <v>23</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E23" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="F23" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -2330,27 +2342,27 @@
         <v>20</v>
       </c>
       <c r="J23" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D24" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E24" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F24" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G24">
         <v>5</v>
@@ -2366,7 +2378,7 @@
         <v>62</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -2374,19 +2386,19 @@
         <v>29</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E25" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G25">
         <v>6</v>
@@ -2402,7 +2414,7 @@
         <v>30</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -2410,19 +2422,19 @@
         <v>31</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E26" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G26">
         <v>2</v>
@@ -2438,7 +2450,7 @@
         <v>32</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -2446,19 +2458,19 @@
         <v>27</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D27" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E27" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G27">
         <v>2</v>
@@ -2474,27 +2486,27 @@
         <v>28</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D28" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E28" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F28" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -2507,10 +2519,10 @@
         <v>2</v>
       </c>
       <c r="J28" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="30">
@@ -2518,19 +2530,19 @@
         <v>33</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D29" t="s">
+        <v>161</v>
+      </c>
+      <c r="E29" t="s">
         <v>164</v>
       </c>
-      <c r="E29" t="s">
-        <v>167</v>
-      </c>
       <c r="F29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G29">
         <v>18</v>
@@ -2546,7 +2558,7 @@
         <v>34</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -2554,16 +2566,16 @@
         <v>20</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -2579,15 +2591,15 @@
         <v>61</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>65</v>
@@ -2607,10 +2619,10 @@
         <v>48</v>
       </c>
       <c r="J31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -2618,7 +2630,7 @@
         <v>24</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D32" t="s">
         <v>65</v>
@@ -2638,18 +2650,18 @@
         <v>10</v>
       </c>
       <c r="J32" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>71</v>
@@ -2671,10 +2683,10 @@
         <v>36</v>
       </c>
       <c r="J33" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -2682,7 +2694,7 @@
         <v>35</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>65</v>
@@ -2704,7 +2716,7 @@
         <v>36</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -2712,13 +2724,13 @@
         <v>37</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J35" t="s">
         <v>38</v>
       </c>
       <c r="K35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -2726,13 +2738,13 @@
         <v>39</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J36" t="s">
         <v>40</v>
       </c>
       <c r="K36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -2740,13 +2752,13 @@
         <v>41</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J37" t="s">
         <v>42</v>
       </c>
       <c r="K37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -2839,19 +2851,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="D4" t="s">
+        <v>238</v>
+      </c>
+      <c r="E4" t="s">
         <v>239</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="F4" t="s">
         <v>240</v>
-      </c>
-      <c r="D4" t="s">
-        <v>241</v>
-      </c>
-      <c r="E4" t="s">
-        <v>242</v>
-      </c>
-      <c r="F4" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2936,7 +2948,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -2981,7 +2993,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B15">
         <v>0.5</v>
@@ -3001,7 +3013,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B17" s="10">
         <f>B11+B11*B15</f>
@@ -3026,7 +3038,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B18">
         <v>0.5</v>
@@ -3046,7 +3058,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B20">
         <f>B17+B17*B18</f>
@@ -3095,22 +3107,22 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B2" s="8">
         <f>SUMIF(BOM!B2:B37,"=SMT",BOM!G2:G37)</f>
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B3" s="8">
         <f>SUMIF(BOM!B3:B38,"=TH",BOM!G3:G38)</f>
@@ -3123,13 +3135,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B5" s="8"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B6" s="8">
         <v>148</v>
@@ -3137,7 +3149,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B7" s="8">
         <v>115</v>
@@ -3145,7 +3157,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B9">
         <f>COUNT(BOM!G2:G37)</f>
@@ -3154,11 +3166,11 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B10">
         <f>SUM(BOM!G2:G38)</f>
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -3206,7 +3218,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -3217,7 +3229,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3228,7 +3240,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -3239,13 +3251,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3261,7 +3273,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C7">
         <v>25</v>
@@ -3272,7 +3284,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C8">
         <v>13</v>
@@ -3289,7 +3301,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -3300,7 +3312,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3311,7 +3323,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3322,7 +3334,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3333,7 +3345,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3344,7 +3356,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3355,7 +3367,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3366,7 +3378,7 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3377,7 +3389,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3388,7 +3400,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3448,13 +3460,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -3465,7 +3477,7 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -3494,7 +3506,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C1" t="s">
         <v>45</v>
@@ -3514,10 +3526,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D30" si="0">IF(A3=C3, "equal", "not")</f>
@@ -3538,10 +3550,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -3550,10 +3562,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -3562,10 +3574,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -3574,10 +3586,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -3586,10 +3598,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
@@ -3598,10 +3610,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -3610,10 +3622,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -3622,10 +3634,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
@@ -3646,10 +3658,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
@@ -3670,10 +3682,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -3694,10 +3706,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -3730,10 +3742,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
@@ -3742,10 +3754,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C22" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
@@ -3754,10 +3766,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C23" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
@@ -3766,10 +3778,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
@@ -3778,10 +3790,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
@@ -3790,10 +3802,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
@@ -3802,10 +3814,10 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
@@ -3814,10 +3826,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C28" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -3826,10 +3838,10 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
@@ -3838,10 +3850,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -3883,20 +3895,20 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="C2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="B3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -3919,7 +3931,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B5" s="12">
         <v>650</v>
@@ -3948,7 +3960,7 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B6">
         <v>100</v>
@@ -4006,7 +4018,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="13" customFormat="1" ht="23">
       <c r="A1" s="26" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="14"/>
@@ -4020,10 +4032,10 @@
     </row>
     <row r="3" spans="1:10" s="23" customFormat="1">
       <c r="A3" s="23" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>0</v>
@@ -4041,7 +4053,7 @@
         <v>45</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="I3" s="23" t="s">
         <v>3</v>
@@ -4058,22 +4070,22 @@
         <v>12</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H4" s="15">
         <v>1</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="18" customFormat="1" ht="30">
@@ -4084,22 +4096,22 @@
         <v>15</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E5" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="F5" s="19" t="s">
-        <v>152</v>
-      </c>
       <c r="G5" s="19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H5" s="18">
         <v>1</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -4110,16 +4122,16 @@
         <v>16</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H6" s="15">
         <v>1</v>
@@ -4136,16 +4148,16 @@
         <v>13</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H7" s="18">
         <v>1</v>
@@ -4162,16 +4174,16 @@
         <v>14</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H8" s="15">
         <v>1</v>
@@ -4189,13 +4201,13 @@
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="19" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H9" s="18">
         <v>2</v>
@@ -4212,16 +4224,16 @@
         <v>18</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H10" s="15">
         <v>1</v>
@@ -4238,22 +4250,22 @@
         <v>17</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H11" s="18">
         <v>2</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -4267,10 +4279,10 @@
         <v>71</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G12" s="16" t="s">
         <v>51</v>
@@ -4287,19 +4299,19 @@
         <v>10</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>73</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="H13" s="18">
         <v>2</v>
@@ -4319,10 +4331,10 @@
         <v>72</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G14" s="16" t="s">
         <v>85</v>
@@ -4339,16 +4351,16 @@
         <v>12</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>71</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G15" s="19" t="s">
         <v>58</v>
@@ -4365,25 +4377,25 @@
         <v>13</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>71</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="H16" s="15">
         <v>2</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="2:10" s="18" customFormat="1" ht="60">
@@ -4391,16 +4403,16 @@
         <v>14</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>71</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G17" s="19" t="s">
         <v>56</v>
@@ -4423,13 +4435,13 @@
         <v>71</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H18" s="15">
         <v>4</v>
@@ -4443,16 +4455,16 @@
         <v>16</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D19" s="19" t="s">
         <v>71</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G19" s="19" t="s">
         <v>54</v>
@@ -4475,10 +4487,10 @@
         <v>72</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G20" s="16" t="s">
         <v>82</v>
@@ -4501,10 +4513,10 @@
         <v>71</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>77</v>
@@ -4524,17 +4536,17 @@
         <v>19</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D22" s="16"/>
       <c r="E22" s="15" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="H22" s="15">
         <v>5</v>
@@ -4554,13 +4566,13 @@
         <v>71</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H23" s="18">
         <v>6</v>
@@ -4580,13 +4592,13 @@
         <v>71</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H24" s="15">
         <v>2</v>
@@ -4606,13 +4618,13 @@
         <v>71</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H25" s="18">
         <v>2</v>
@@ -4626,25 +4638,25 @@
         <v>23</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D26" s="16" t="s">
         <v>71</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G26" s="15" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="H26" s="15">
         <v>1</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="2:10" s="18" customFormat="1" ht="45">
@@ -4658,13 +4670,13 @@
         <v>71</v>
       </c>
       <c r="E27" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="F27" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="F27" s="18" t="s">
-        <v>167</v>
-      </c>
       <c r="G27" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H27" s="18">
         <v>18</v>
@@ -4682,13 +4694,13 @@
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H28" s="15">
         <v>1</v>
@@ -4702,7 +4714,7 @@
         <v>26</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D29" s="19"/>
       <c r="E29" s="19" t="s">
@@ -4716,7 +4728,7 @@
         <v>6</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="2:10">
@@ -4738,7 +4750,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="2:10" s="18" customFormat="1">
@@ -4746,7 +4758,7 @@
         <v>28</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="18" t="s">
@@ -4759,7 +4771,7 @@
         <v>1</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="2:10">
@@ -4792,13 +4804,13 @@
       </c>
       <c r="D33" s="19"/>
       <c r="E33" s="18" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="H33" s="18">
         <v>1</v>
@@ -4816,19 +4828,19 @@
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="15" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H34" s="15">
         <v>1</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="35" spans="2:9" s="18" customFormat="1">
@@ -4840,19 +4852,19 @@
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="18" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F35" s="18" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H35" s="18">
         <v>1</v>
       </c>
       <c r="I35" s="18" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="2:9">
@@ -4864,19 +4876,19 @@
       </c>
       <c r="D36" s="16"/>
       <c r="E36" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G36" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H36" s="15">
         <v>1</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="2:9">

</xml_diff>